<commit_message>
finally fixed the tests
</commit_message>
<xml_diff>
--- a/server/src/static/example.xlsx
+++ b/server/src/static/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="23360" windowHeight="13820" tabRatio="863" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="23360" windowHeight="13820" tabRatio="863" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="22" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="166">
   <si>
     <t>Programs for men who have sex with men</t>
   </si>
@@ -564,7 +564,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -687,8 +687,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF16365C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,8 +741,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -758,6 +786,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1425,7 +1481,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1552,6 +1608,26 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="663" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="664">
@@ -4785,8 +4861,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10547,7 +10623,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11558,7 +11634,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -14812,10 +14888,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -15161,285 +15237,155 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="18" customFormat="1">
-      <c r="B14" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
-        <v>MSM</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="5" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="60">
+        <v>0.3</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="60">
+        <v>0.25</v>
+      </c>
+      <c r="G14" s="61"/>
+      <c r="H14" s="60">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="60">
+        <v>0.2</v>
+      </c>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="T14" s="29"/>
-    </row>
-    <row r="15" spans="1:20" s="18" customFormat="1">
-      <c r="B15" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="5" t="s">
+      <c r="T14" s="63"/>
+    </row>
+    <row r="16" spans="1:20" s="18" customFormat="1">
+      <c r="B16" s="6"/>
+      <c r="T16" s="31"/>
+    </row>
+    <row r="17" spans="1:20" s="18" customFormat="1">
+      <c r="B17" s="6"/>
+      <c r="T17" s="31"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="13"/>
+      <c r="C19" s="14">
+        <v>2000</v>
+      </c>
+      <c r="D19" s="14">
+        <v>2001</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2002</v>
+      </c>
+      <c r="F19" s="14">
+        <v>2003</v>
+      </c>
+      <c r="G19" s="14">
+        <v>2004</v>
+      </c>
+      <c r="H19" s="14">
+        <v>2005</v>
+      </c>
+      <c r="I19" s="14">
+        <v>2006</v>
+      </c>
+      <c r="J19" s="14">
+        <v>2007</v>
+      </c>
+      <c r="K19" s="14">
+        <v>2008</v>
+      </c>
+      <c r="L19" s="14">
+        <v>2009</v>
+      </c>
+      <c r="M19" s="14">
+        <v>2010</v>
+      </c>
+      <c r="N19" s="14">
+        <v>2011</v>
+      </c>
+      <c r="O19" s="14">
+        <v>2012</v>
+      </c>
+      <c r="P19" s="14">
+        <v>2013</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>2014</v>
+      </c>
+      <c r="R19" s="14">
+        <v>2015</v>
+      </c>
+      <c r="S19" s="13"/>
+      <c r="T19" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="13"/>
+      <c r="B20" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38">
+        <v>50</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38">
+        <v>70</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38">
+        <v>190</v>
+      </c>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="T15" s="29"/>
-    </row>
-    <row r="16" spans="1:20" s="18" customFormat="1">
-      <c r="B16" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>Male PWID</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="25">
-        <v>0.3</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="G16" s="22"/>
-      <c r="H16" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T16" s="29"/>
-    </row>
-    <row r="17" spans="1:20" s="18" customFormat="1">
-      <c r="B17" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>Other males</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T17" s="29"/>
-    </row>
-    <row r="18" spans="1:20" s="18" customFormat="1">
-      <c r="B18" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other females</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T18" s="29"/>
-    </row>
-    <row r="19" spans="1:20" s="18" customFormat="1">
-      <c r="B19" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
-        <v>Clients</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T19" s="29"/>
-    </row>
-    <row r="21" spans="1:20" s="18" customFormat="1">
-      <c r="B21" s="6"/>
-      <c r="T21" s="31"/>
-    </row>
-    <row r="22" spans="1:20" s="18" customFormat="1">
-      <c r="B22" s="6"/>
-      <c r="T22" s="31"/>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="13"/>
-      <c r="C24" s="14">
-        <v>2000</v>
-      </c>
-      <c r="D24" s="14">
-        <v>2001</v>
-      </c>
-      <c r="E24" s="14">
-        <v>2002</v>
-      </c>
-      <c r="F24" s="14">
-        <v>2003</v>
-      </c>
-      <c r="G24" s="14">
-        <v>2004</v>
-      </c>
-      <c r="H24" s="14">
-        <v>2005</v>
-      </c>
-      <c r="I24" s="14">
-        <v>2006</v>
-      </c>
-      <c r="J24" s="14">
-        <v>2007</v>
-      </c>
-      <c r="K24" s="14">
-        <v>2008</v>
-      </c>
-      <c r="L24" s="14">
-        <v>2009</v>
-      </c>
-      <c r="M24" s="14">
-        <v>2010</v>
-      </c>
-      <c r="N24" s="14">
-        <v>2011</v>
-      </c>
-      <c r="O24" s="14">
-        <v>2012</v>
-      </c>
-      <c r="P24" s="14">
-        <v>2013</v>
-      </c>
-      <c r="Q24" s="14">
-        <v>2014</v>
-      </c>
-      <c r="R24" s="14">
-        <v>2015</v>
-      </c>
-      <c r="S24" s="13"/>
-      <c r="T24" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="13"/>
-      <c r="B25" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38">
-        <v>50</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38">
-        <v>70</v>
-      </c>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38">
-        <v>190</v>
-      </c>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T25" s="38"/>
+      <c r="T20" s="38"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>

</xml_diff>

<commit_message>
couple more fixes after running tests
</commit_message>
<xml_diff>
--- a/server/src/static/example.xlsx
+++ b/server/src/static/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="2235" windowWidth="23355" windowHeight="13815" tabRatio="863" activeTab="1"/>
+    <workbookView xWindow="2235" yWindow="2235" windowWidth="23355" windowHeight="13815" tabRatio="863" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="22" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="166">
   <si>
     <t>Programs for men who have sex with men</t>
   </si>
@@ -564,7 +564,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -696,21 +696,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF16365C"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -755,7 +740,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -794,21 +779,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
@@ -1488,7 +1458,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="655" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1613,24 +1583,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="663" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="19" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="21" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="663" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2621,15 +2577,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="58" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
+      <c r="A2" s="58"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
@@ -3972,9 +3928,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64:E65"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4868,8 +4822,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7551,7 +7505,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -11641,7 +11595,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -13007,10 +12961,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T74"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13788,171 +13742,164 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C31" s="22"/>
-      <c r="D31" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="25">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H31" s="25">
-        <v>0.17</v>
-      </c>
-      <c r="I31" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="J31" s="22"/>
-      <c r="K31" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="L31" s="22"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="25">
-        <v>0.39</v>
-      </c>
-      <c r="O31" s="22"/>
-      <c r="P31" s="25">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="22"/>
+    <row r="31" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T31" s="31"/>
     </row>
     <row r="32" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="27">
-        <f>550000*D31</f>
-        <v>11000</v>
-      </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27">
-        <f t="shared" ref="G32:P32" si="0">550000*G31</f>
-        <v>77000.000000000015</v>
-      </c>
-      <c r="H32" s="27">
-        <f t="shared" si="0"/>
-        <v>93500</v>
-      </c>
-      <c r="I32" s="27">
-        <f t="shared" si="0"/>
-        <v>27500</v>
-      </c>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27">
-        <f t="shared" si="0"/>
-        <v>110000</v>
-      </c>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27">
-        <f t="shared" si="0"/>
-        <v>214500</v>
-      </c>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27">
-        <f t="shared" si="0"/>
-        <v>154000.00000000003</v>
-      </c>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
       <c r="T32" s="31"/>
     </row>
     <row r="33" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="T34" s="31"/>
-    </row>
-    <row r="35" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
-      <c r="T35" s="31"/>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="C35" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D35" s="12">
+        <v>2001</v>
+      </c>
+      <c r="E35" s="12">
+        <v>2002</v>
+      </c>
+      <c r="F35" s="12">
+        <v>2003</v>
+      </c>
+      <c r="G35" s="12">
+        <v>2004</v>
+      </c>
+      <c r="H35" s="12">
+        <v>2005</v>
+      </c>
+      <c r="I35" s="12">
+        <v>2006</v>
+      </c>
+      <c r="J35" s="12">
+        <v>2007</v>
+      </c>
+      <c r="K35" s="12">
+        <v>2008</v>
+      </c>
+      <c r="L35" s="12">
+        <v>2009</v>
+      </c>
+      <c r="M35" s="12">
+        <v>2010</v>
+      </c>
+      <c r="N35" s="12">
+        <v>2011</v>
+      </c>
+      <c r="O35" s="12">
+        <v>2012</v>
+      </c>
+      <c r="P35" s="12">
+        <v>2013</v>
+      </c>
+      <c r="Q35" s="12">
+        <v>2014</v>
+      </c>
+      <c r="R35" s="12">
+        <v>2015</v>
+      </c>
+      <c r="S35" s="11"/>
+      <c r="T35" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>MSM</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T36" s="30">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="C37" s="12">
-        <v>2000</v>
-      </c>
-      <c r="D37" s="12">
-        <v>2001</v>
-      </c>
-      <c r="E37" s="12">
-        <v>2002</v>
-      </c>
-      <c r="F37" s="12">
-        <v>2003</v>
-      </c>
-      <c r="G37" s="12">
-        <v>2004</v>
-      </c>
-      <c r="H37" s="12">
-        <v>2005</v>
-      </c>
-      <c r="I37" s="12">
-        <v>2006</v>
-      </c>
-      <c r="J37" s="12">
-        <v>2007</v>
-      </c>
-      <c r="K37" s="12">
-        <v>2008</v>
-      </c>
-      <c r="L37" s="12">
-        <v>2009</v>
-      </c>
-      <c r="M37" s="12">
-        <v>2010</v>
-      </c>
-      <c r="N37" s="12">
-        <v>2011</v>
-      </c>
-      <c r="O37" s="12">
-        <v>2012</v>
-      </c>
-      <c r="P37" s="12">
-        <v>2013</v>
-      </c>
-      <c r="Q37" s="12">
-        <v>2014</v>
-      </c>
-      <c r="R37" s="12">
-        <v>2015</v>
-      </c>
-      <c r="S37" s="11"/>
-      <c r="T37" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B37" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="25">
+        <v>0.24</v>
+      </c>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="25">
+        <v>0.27</v>
+      </c>
+      <c r="M37" s="22"/>
+      <c r="N37" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="O37" s="22"/>
+      <c r="P37" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T37" s="30"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
-        <v>MSM</v>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Male PWID</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
@@ -13974,51 +13921,43 @@
         <v>54</v>
       </c>
       <c r="T38" s="30">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW</v>
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Other males</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
-      <c r="F39" s="25">
-        <v>0.2</v>
-      </c>
+      <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="25">
-        <v>0.24</v>
-      </c>
+      <c r="I39" s="22"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
-      <c r="L39" s="25">
-        <v>0.27</v>
-      </c>
+      <c r="L39" s="22"/>
       <c r="M39" s="22"/>
-      <c r="N39" s="25">
-        <v>0.3</v>
-      </c>
+      <c r="N39" s="22"/>
       <c r="O39" s="22"/>
-      <c r="P39" s="25">
-        <v>0.3</v>
-      </c>
+      <c r="P39" s="22"/>
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T39" s="30"/>
+      <c r="T39" s="30">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>Male PWID</v>
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other females</v>
       </c>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
@@ -14046,8 +13985,8 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>Other males</v>
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>Clients</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -14069,157 +14008,165 @@
         <v>54</v>
       </c>
       <c r="T41" s="30">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other females</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="5" t="s">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="6"/>
+      <c r="T43" s="31"/>
+    </row>
+    <row r="44" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+      <c r="T44" s="31"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="C46" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D46" s="12">
+        <v>2001</v>
+      </c>
+      <c r="E46" s="12">
+        <v>2002</v>
+      </c>
+      <c r="F46" s="12">
+        <v>2003</v>
+      </c>
+      <c r="G46" s="12">
+        <v>2004</v>
+      </c>
+      <c r="H46" s="12">
+        <v>2005</v>
+      </c>
+      <c r="I46" s="12">
+        <v>2006</v>
+      </c>
+      <c r="J46" s="12">
+        <v>2007</v>
+      </c>
+      <c r="K46" s="12">
+        <v>2008</v>
+      </c>
+      <c r="L46" s="12">
+        <v>2009</v>
+      </c>
+      <c r="M46" s="12">
+        <v>2010</v>
+      </c>
+      <c r="N46" s="12">
+        <v>2011</v>
+      </c>
+      <c r="O46" s="12">
+        <v>2012</v>
+      </c>
+      <c r="P46" s="12">
+        <v>2013</v>
+      </c>
+      <c r="Q46" s="12">
+        <v>2014</v>
+      </c>
+      <c r="R46" s="12">
+        <v>2015</v>
+      </c>
+      <c r="S46" s="11"/>
+      <c r="T46" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>MSM</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T42" s="30">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
-        <v>Clients</v>
-      </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22"/>
-      <c r="S43" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T43" s="30">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="6"/>
-      <c r="T45" s="31"/>
-    </row>
-    <row r="46" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="6"/>
-      <c r="T46" s="31"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
+      <c r="T47" s="30">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
-      <c r="C48" s="12">
-        <v>2000</v>
-      </c>
-      <c r="D48" s="12">
-        <v>2001</v>
-      </c>
-      <c r="E48" s="12">
-        <v>2002</v>
-      </c>
-      <c r="F48" s="12">
-        <v>2003</v>
-      </c>
-      <c r="G48" s="12">
-        <v>2004</v>
-      </c>
-      <c r="H48" s="12">
-        <v>2005</v>
-      </c>
-      <c r="I48" s="12">
-        <v>2006</v>
-      </c>
-      <c r="J48" s="12">
-        <v>2007</v>
-      </c>
-      <c r="K48" s="12">
-        <v>2008</v>
-      </c>
-      <c r="L48" s="12">
-        <v>2009</v>
-      </c>
-      <c r="M48" s="12">
-        <v>2010</v>
-      </c>
-      <c r="N48" s="12">
-        <v>2011</v>
-      </c>
-      <c r="O48" s="12">
-        <v>2012</v>
-      </c>
-      <c r="P48" s="12">
-        <v>2013</v>
-      </c>
-      <c r="Q48" s="12">
-        <v>2014</v>
-      </c>
-      <c r="R48" s="12">
-        <v>2015</v>
-      </c>
-      <c r="S48" s="11"/>
-      <c r="T48" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B48" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="25">
+        <v>0.94</v>
+      </c>
+      <c r="M48" s="22"/>
+      <c r="N48" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="O48" s="22"/>
+      <c r="P48" s="25">
+        <v>0.96</v>
+      </c>
+      <c r="Q48" s="22"/>
+      <c r="R48" s="22"/>
+      <c r="S48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T48" s="30"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
-        <v>MSM</v>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Male PWID</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
@@ -14241,39 +14188,35 @@
         <v>54</v>
       </c>
       <c r="T49" s="30">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW</v>
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Other males</v>
       </c>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
-      <c r="F50" s="25">
-        <v>0.8</v>
-      </c>
+      <c r="F50" s="22"/>
       <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="25">
-        <v>0.85</v>
-      </c>
+      <c r="H50" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="I50" s="22"/>
       <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="25">
-        <v>0.94</v>
-      </c>
+      <c r="K50" s="25">
+        <v>0.37</v>
+      </c>
+      <c r="L50" s="22"/>
       <c r="M50" s="22"/>
       <c r="N50" s="25">
-        <v>0.91</v>
+        <v>0.42</v>
       </c>
       <c r="O50" s="22"/>
-      <c r="P50" s="25">
-        <v>0.96</v>
-      </c>
+      <c r="P50" s="22"/>
       <c r="Q50" s="22"/>
       <c r="R50" s="22"/>
       <c r="S50" s="5" t="s">
@@ -14284,21 +14227,27 @@
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>Male PWID</v>
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other females</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
+      <c r="H51" s="25">
+        <v>0.4</v>
+      </c>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
+      <c r="K51" s="25">
+        <v>0.37</v>
+      </c>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
+      <c r="N51" s="25">
+        <v>0.42</v>
+      </c>
       <c r="O51" s="22"/>
       <c r="P51" s="22"/>
       <c r="Q51" s="22"/>
@@ -14306,34 +14255,26 @@
       <c r="S51" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T51" s="30">
-        <v>0.5</v>
-      </c>
+      <c r="T51" s="30"/>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>Other males</v>
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>Clients</v>
       </c>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
-      <c r="H52" s="25">
-        <v>0.4</v>
-      </c>
+      <c r="H52" s="22"/>
       <c r="I52" s="22"/>
       <c r="J52" s="22"/>
-      <c r="K52" s="25">
-        <v>0.37</v>
-      </c>
+      <c r="K52" s="22"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
-      <c r="N52" s="25">
-        <v>0.42</v>
-      </c>
+      <c r="N52" s="22"/>
       <c r="O52" s="22"/>
       <c r="P52" s="22"/>
       <c r="Q52" s="22"/>
@@ -14341,160 +14282,166 @@
       <c r="S52" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T52" s="30"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other females</v>
-      </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="25">
-        <v>0.37</v>
-      </c>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="25">
-        <v>0.42</v>
-      </c>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="5" t="s">
+      <c r="T52" s="30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="6"/>
+      <c r="T54" s="31"/>
+    </row>
+    <row r="55" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="6"/>
+      <c r="T55" s="31"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="C57" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D57" s="12">
+        <v>2001</v>
+      </c>
+      <c r="E57" s="12">
+        <v>2002</v>
+      </c>
+      <c r="F57" s="12">
+        <v>2003</v>
+      </c>
+      <c r="G57" s="12">
+        <v>2004</v>
+      </c>
+      <c r="H57" s="12">
+        <v>2005</v>
+      </c>
+      <c r="I57" s="12">
+        <v>2006</v>
+      </c>
+      <c r="J57" s="12">
+        <v>2007</v>
+      </c>
+      <c r="K57" s="12">
+        <v>2008</v>
+      </c>
+      <c r="L57" s="12">
+        <v>2009</v>
+      </c>
+      <c r="M57" s="12">
+        <v>2010</v>
+      </c>
+      <c r="N57" s="12">
+        <v>2011</v>
+      </c>
+      <c r="O57" s="12">
+        <v>2012</v>
+      </c>
+      <c r="P57" s="12">
+        <v>2013</v>
+      </c>
+      <c r="Q57" s="12">
+        <v>2014</v>
+      </c>
+      <c r="R57" s="12">
+        <v>2015</v>
+      </c>
+      <c r="S57" s="11"/>
+      <c r="T57" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>MSM</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T53" s="30"/>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
-        <v>Clients</v>
-      </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-      <c r="S54" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T54" s="30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="6"/>
-      <c r="T56" s="31"/>
-    </row>
-    <row r="57" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="6"/>
-      <c r="T57" s="31"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="11"/>
+      <c r="T58" s="29">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
-      <c r="C59" s="12">
-        <v>2000</v>
-      </c>
-      <c r="D59" s="12">
-        <v>2001</v>
-      </c>
-      <c r="E59" s="12">
-        <v>2002</v>
-      </c>
-      <c r="F59" s="12">
-        <v>2003</v>
-      </c>
-      <c r="G59" s="12">
-        <v>2004</v>
-      </c>
-      <c r="H59" s="12">
-        <v>2005</v>
-      </c>
-      <c r="I59" s="12">
-        <v>2006</v>
-      </c>
-      <c r="J59" s="12">
-        <v>2007</v>
-      </c>
-      <c r="K59" s="12">
-        <v>2008</v>
-      </c>
-      <c r="L59" s="12">
-        <v>2009</v>
-      </c>
-      <c r="M59" s="12">
-        <v>2010</v>
-      </c>
-      <c r="N59" s="12">
-        <v>2011</v>
-      </c>
-      <c r="O59" s="12">
-        <v>2012</v>
-      </c>
-      <c r="P59" s="12">
-        <v>2013</v>
-      </c>
-      <c r="Q59" s="12">
-        <v>2014</v>
-      </c>
-      <c r="R59" s="12">
-        <v>2015</v>
-      </c>
-      <c r="S59" s="11"/>
-      <c r="T59" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B59" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW</v>
+      </c>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="25">
+        <v>0.84</v>
+      </c>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="25">
+        <v>0.89</v>
+      </c>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="25">
+        <v>0.96</v>
+      </c>
+      <c r="M59" s="22"/>
+      <c r="N59" s="25">
+        <v>0.94</v>
+      </c>
+      <c r="O59" s="22"/>
+      <c r="P59" s="25">
+        <v>0.98</v>
+      </c>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
+      <c r="S59" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T59" s="38"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
-        <v>MSM</v>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Male PWID</v>
       </c>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
@@ -14515,52 +14462,44 @@
       <c r="S60" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T60" s="29">
+      <c r="T60" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW</v>
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Other males</v>
       </c>
       <c r="C61" s="22"/>
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
-      <c r="F61" s="25">
-        <v>0.84</v>
-      </c>
+      <c r="F61" s="22"/>
       <c r="G61" s="22"/>
       <c r="H61" s="22"/>
-      <c r="I61" s="25">
-        <v>0.89</v>
-      </c>
+      <c r="I61" s="22"/>
       <c r="J61" s="22"/>
       <c r="K61" s="22"/>
-      <c r="L61" s="25">
-        <v>0.96</v>
-      </c>
+      <c r="L61" s="22"/>
       <c r="M61" s="22"/>
-      <c r="N61" s="25">
-        <v>0.94</v>
-      </c>
+      <c r="N61" s="22"/>
       <c r="O61" s="22"/>
-      <c r="P61" s="25">
-        <v>0.98</v>
-      </c>
+      <c r="P61" s="22"/>
       <c r="Q61" s="22"/>
       <c r="R61" s="22"/>
       <c r="S61" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T61" s="38"/>
+      <c r="T61" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>Male PWID</v>
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other females</v>
       </c>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
@@ -14581,195 +14520,195 @@
       <c r="S62" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T62" s="30">
+      <c r="T62" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>Other males</v>
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>Clients</v>
       </c>
       <c r="C63" s="22"/>
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
+      <c r="F63" s="25">
+        <v>0.84</v>
+      </c>
       <c r="G63" s="22"/>
       <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
+      <c r="I63" s="25">
+        <v>0.89</v>
+      </c>
       <c r="J63" s="22"/>
       <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
+      <c r="L63" s="25">
+        <v>0.96</v>
+      </c>
       <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
+      <c r="N63" s="25">
+        <v>0.94</v>
+      </c>
       <c r="O63" s="22"/>
-      <c r="P63" s="22"/>
+      <c r="P63" s="25">
+        <v>0.98</v>
+      </c>
       <c r="Q63" s="22"/>
       <c r="R63" s="22"/>
       <c r="S63" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T63" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other females</v>
-      </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="5" t="s">
+      <c r="T63" s="39"/>
+    </row>
+    <row r="65" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="6"/>
+      <c r="T65" s="31"/>
+    </row>
+    <row r="66" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="6"/>
+      <c r="T66" s="31"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+      <c r="P67" s="11"/>
+      <c r="Q67" s="11"/>
+      <c r="R67" s="11"/>
+      <c r="S67" s="11"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="C68" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D68" s="12">
+        <v>2001</v>
+      </c>
+      <c r="E68" s="12">
+        <v>2002</v>
+      </c>
+      <c r="F68" s="12">
+        <v>2003</v>
+      </c>
+      <c r="G68" s="12">
+        <v>2004</v>
+      </c>
+      <c r="H68" s="12">
+        <v>2005</v>
+      </c>
+      <c r="I68" s="12">
+        <v>2006</v>
+      </c>
+      <c r="J68" s="12">
+        <v>2007</v>
+      </c>
+      <c r="K68" s="12">
+        <v>2008</v>
+      </c>
+      <c r="L68" s="12">
+        <v>2009</v>
+      </c>
+      <c r="M68" s="12">
+        <v>2010</v>
+      </c>
+      <c r="N68" s="12">
+        <v>2011</v>
+      </c>
+      <c r="O68" s="12">
+        <v>2012</v>
+      </c>
+      <c r="P68" s="12">
+        <v>2013</v>
+      </c>
+      <c r="Q68" s="12">
+        <v>2014</v>
+      </c>
+      <c r="R68" s="12">
+        <v>2015</v>
+      </c>
+      <c r="S68" s="11"/>
+      <c r="T68" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>MSM</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="22"/>
+      <c r="K69" s="22"/>
+      <c r="L69" s="22"/>
+      <c r="M69" s="22"/>
+      <c r="N69" s="22"/>
+      <c r="O69" s="22"/>
+      <c r="P69" s="22"/>
+      <c r="Q69" s="22"/>
+      <c r="R69" s="22"/>
+      <c r="S69" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T64" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
-      <c r="B65" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
-        <v>Clients</v>
-      </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="25">
-        <v>0.84</v>
-      </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="25">
-        <v>0.89</v>
-      </c>
-      <c r="J65" s="22"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="25">
-        <v>0.96</v>
-      </c>
-      <c r="M65" s="22"/>
-      <c r="N65" s="25">
-        <v>0.94</v>
-      </c>
-      <c r="O65" s="22"/>
-      <c r="P65" s="25">
-        <v>0.98</v>
-      </c>
-      <c r="Q65" s="22"/>
-      <c r="R65" s="22"/>
-      <c r="S65" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T65" s="39"/>
-    </row>
-    <row r="67" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="6"/>
-      <c r="T67" s="31"/>
-    </row>
-    <row r="68" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="6"/>
-      <c r="T68" s="31"/>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
+      <c r="T69" s="50">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
-      <c r="C70" s="12">
-        <v>2000</v>
-      </c>
-      <c r="D70" s="12">
-        <v>2001</v>
-      </c>
-      <c r="E70" s="12">
-        <v>2002</v>
-      </c>
-      <c r="F70" s="12">
-        <v>2003</v>
-      </c>
-      <c r="G70" s="12">
-        <v>2004</v>
-      </c>
-      <c r="H70" s="12">
-        <v>2005</v>
-      </c>
-      <c r="I70" s="12">
-        <v>2006</v>
-      </c>
-      <c r="J70" s="12">
-        <v>2007</v>
-      </c>
-      <c r="K70" s="12">
-        <v>2008</v>
-      </c>
-      <c r="L70" s="12">
-        <v>2009</v>
-      </c>
-      <c r="M70" s="12">
-        <v>2010</v>
-      </c>
-      <c r="N70" s="12">
-        <v>2011</v>
-      </c>
-      <c r="O70" s="12">
-        <v>2012</v>
-      </c>
-      <c r="P70" s="12">
-        <v>2013</v>
-      </c>
-      <c r="Q70" s="12">
-        <v>2014</v>
-      </c>
-      <c r="R70" s="12">
-        <v>2015</v>
-      </c>
-      <c r="S70" s="11"/>
-      <c r="T70" s="4" t="s">
-        <v>32</v>
+      <c r="B70" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Male PWID</v>
+      </c>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="22"/>
+      <c r="K70" s="22"/>
+      <c r="L70" s="22"/>
+      <c r="M70" s="22"/>
+      <c r="N70" s="22"/>
+      <c r="O70" s="22"/>
+      <c r="P70" s="22"/>
+      <c r="Q70" s="22"/>
+      <c r="R70" s="22"/>
+      <c r="S70" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T70" s="50">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$3</f>
-        <v>MSM</v>
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Other males</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
@@ -14797,8 +14736,8 @@
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>Male PWID</v>
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>Clients</v>
       </c>
       <c r="C72" s="22"/>
       <c r="D72" s="22"/>
@@ -14820,64 +14759,6 @@
         <v>54</v>
       </c>
       <c r="T72" s="50">
-        <v>2.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>Other males</v>
-      </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
-      <c r="G73" s="22"/>
-      <c r="H73" s="22"/>
-      <c r="I73" s="22"/>
-      <c r="J73" s="22"/>
-      <c r="K73" s="22"/>
-      <c r="L73" s="22"/>
-      <c r="M73" s="22"/>
-      <c r="N73" s="22"/>
-      <c r="O73" s="22"/>
-      <c r="P73" s="22"/>
-      <c r="Q73" s="22"/>
-      <c r="R73" s="22"/>
-      <c r="S73" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T73" s="50">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$8</f>
-        <v>Clients</v>
-      </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
-      <c r="K74" s="22"/>
-      <c r="L74" s="22"/>
-      <c r="M74" s="22"/>
-      <c r="N74" s="22"/>
-      <c r="O74" s="22"/>
-      <c r="P74" s="22"/>
-      <c r="Q74" s="22"/>
-      <c r="R74" s="22"/>
-      <c r="S74" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T74" s="50">
         <v>0.03</v>
       </c>
     </row>
@@ -14895,9 +14776,11 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15242,155 +15125,295 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59">
+      <c r="B14" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>MSM</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T14" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>Male PWID</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="56">
         <v>0.3</v>
       </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="59">
+      <c r="E16" s="57"/>
+      <c r="F16" s="56">
         <v>0.25</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="59">
+      <c r="G16" s="57"/>
+      <c r="H16" s="56">
         <v>0.2</v>
       </c>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="59">
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="56">
         <v>0.2</v>
       </c>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="61" t="s">
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T14" s="62"/>
-    </row>
-    <row r="16" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="T16" s="31"/>
+      <c r="T16" s="29"/>
     </row>
     <row r="17" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="T17" s="31"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="B17" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>Other males</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T17" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other females</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T18" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$8</f>
+        <v>Clients</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="T21" s="31"/>
+    </row>
+    <row r="22" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="T22" s="31"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="C19" s="14">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="C24" s="14">
         <v>2000</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D24" s="14">
         <v>2001</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E24" s="14">
         <v>2002</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F24" s="14">
         <v>2003</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G24" s="14">
         <v>2004</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H24" s="14">
         <v>2005</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I24" s="14">
         <v>2006</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J24" s="14">
         <v>2007</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K24" s="14">
         <v>2008</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L24" s="14">
         <v>2009</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M24" s="14">
         <v>2010</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N24" s="14">
         <v>2011</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O24" s="14">
         <v>2012</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P24" s="14">
         <v>2013</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q24" s="14">
         <v>2014</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R24" s="14">
         <v>2015</v>
       </c>
-      <c r="S19" s="13"/>
-      <c r="T19" s="4" t="s">
+      <c r="S24" s="13"/>
+      <c r="T24" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="43" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38">
         <v>50</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38">
+      <c r="E25" s="38"/>
+      <c r="F25" s="38">
         <v>70</v>
       </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38">
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38">
         <v>190</v>
       </c>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="5" t="s">
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T20" s="38"/>
+      <c r="T25" s="38"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>

</xml_diff>